<commit_message>
20/11/2017 - Test Data commit
</commit_message>
<xml_diff>
--- a/src/main/resources/config/stage/TestData/TestData.xlsx
+++ b/src/main/resources/config/stage/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7728" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7728" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="S181372" sheetId="1" r:id="rId1"/>
@@ -14,21 +14,21 @@
     <sheet name="HelpDesk" sheetId="15" r:id="rId5"/>
     <sheet name="CurrencyExchangeRates" sheetId="16" r:id="rId6"/>
     <sheet name="CurrencyExchangeRateMapping" sheetId="17" r:id="rId7"/>
-    <sheet name="AccountMaster_S205195" sheetId="7" r:id="rId8"/>
-    <sheet name="AccountHeadMapping_S205175" sheetId="18" r:id="rId9"/>
-    <sheet name="AccountHead_S205168" sheetId="9" r:id="rId10"/>
-    <sheet name="Events Configuration" sheetId="14" r:id="rId11"/>
-    <sheet name="SuspenseAccount_S205193" sheetId="10" r:id="rId12"/>
-    <sheet name="Institute" sheetId="5" r:id="rId13"/>
-    <sheet name="QMRReporting" sheetId="12" r:id="rId14"/>
+    <sheet name="CardHolder" sheetId="19" r:id="rId8"/>
+    <sheet name="AccountMaster_S205195" sheetId="7" r:id="rId9"/>
+    <sheet name="AccountHeadMapping_S205175" sheetId="18" r:id="rId10"/>
+    <sheet name="AccountHead_S205168" sheetId="9" r:id="rId11"/>
+    <sheet name="Events Configuration" sheetId="14" r:id="rId12"/>
+    <sheet name="SuspenseAccount_S205193" sheetId="10" r:id="rId13"/>
+    <sheet name="Institute" sheetId="5" r:id="rId14"/>
+    <sheet name="QMRReporting" sheetId="12" r:id="rId15"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:H25"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1550" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1899" uniqueCount="605">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -1520,6 +1520,330 @@
   </si>
   <si>
     <t>5130003313500015</t>
+  </si>
+  <si>
+    <t>TranSactionType</t>
+  </si>
+  <si>
+    <t>TransactionAmount</t>
+  </si>
+  <si>
+    <t>TransactionCurrency</t>
+  </si>
+  <si>
+    <t>ConversionRate</t>
+  </si>
+  <si>
+    <t>CardNumber</t>
+  </si>
+  <si>
+    <t>TransferAmount</t>
+  </si>
+  <si>
+    <t>CurrencyName</t>
+  </si>
+  <si>
+    <t>ContactNumber</t>
+  </si>
+  <si>
+    <t>TransfererName</t>
+  </si>
+  <si>
+    <t>Memo</t>
+  </si>
+  <si>
+    <t>TransactionPassword</t>
+  </si>
+  <si>
+    <t>TransactionRemarks</t>
+  </si>
+  <si>
+    <t>AmountToTransferWalletToWallet</t>
+  </si>
+  <si>
+    <t>WalletTransferCurrecny</t>
+  </si>
+  <si>
+    <t>WalletNumberFromTransferMoney</t>
+  </si>
+  <si>
+    <t>WalletToWalletTransferSucessMsg</t>
+  </si>
+  <si>
+    <t>NoOfTransactionsCount</t>
+  </si>
+  <si>
+    <t>FromDate</t>
+  </si>
+  <si>
+    <t>ToDate</t>
+  </si>
+  <si>
+    <t>ReplacementResone</t>
+  </si>
+  <si>
+    <t>ReplaceConfirmMessage</t>
+  </si>
+  <si>
+    <t>BlockCardRemark</t>
+  </si>
+  <si>
+    <t>BlockConfirmationMsg</t>
+  </si>
+  <si>
+    <t>UnblockCardRemark</t>
+  </si>
+  <si>
+    <t>UnblockConfirmationMsg</t>
+  </si>
+  <si>
+    <t>WalletActivationRemark</t>
+  </si>
+  <si>
+    <t>WalletDeactivateRemark</t>
+  </si>
+  <si>
+    <t>WalletActivateConfirmMsg</t>
+  </si>
+  <si>
+    <t>WalletDeactivateConfirmMsg</t>
+  </si>
+  <si>
+    <t>eComActivationConfirmMsg</t>
+  </si>
+  <si>
+    <t>beneficiaryID</t>
+  </si>
+  <si>
+    <t>beneficiaryFirstName</t>
+  </si>
+  <si>
+    <t>beneficiaryMiddleName</t>
+  </si>
+  <si>
+    <t>beneficiaryLastName</t>
+  </si>
+  <si>
+    <t>beneficiaryAddressLine1</t>
+  </si>
+  <si>
+    <t>beneficiaryAddressLine2</t>
+  </si>
+  <si>
+    <t>beneficiaryAddressLine3</t>
+  </si>
+  <si>
+    <t>beneficiaryCountryName</t>
+  </si>
+  <si>
+    <t>beneficiaryStateName</t>
+  </si>
+  <si>
+    <t>beneficiaryCityName</t>
+  </si>
+  <si>
+    <t>beneficiaryZIPCode</t>
+  </si>
+  <si>
+    <t>beneficiaryEmailAddress</t>
+  </si>
+  <si>
+    <t>beneficiaryMobileNumber</t>
+  </si>
+  <si>
+    <t>beneficiaryRemittanceAamount</t>
+  </si>
+  <si>
+    <t>beneficiaryRemittanceCurrency</t>
+  </si>
+  <si>
+    <t>newPassword</t>
+  </si>
+  <si>
+    <t>CardHolderTransPassword</t>
+  </si>
+  <si>
+    <t>FirstSequrityQuestion</t>
+  </si>
+  <si>
+    <t>FirstSequrityAnswer</t>
+  </si>
+  <si>
+    <t>SecondSequrityQuestion</t>
+  </si>
+  <si>
+    <t>SecondSequrityAnswer</t>
+  </si>
+  <si>
+    <t>TC_walletToWalletTransfer</t>
+  </si>
+  <si>
+    <t>https://stage.sa.cardholder.mastercard.com/mpts/eis/app</t>
+  </si>
+  <si>
+    <t>10000172850000001</t>
+  </si>
+  <si>
+    <t>qweR@1234</t>
+  </si>
+  <si>
+    <t>Fund Transfer</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>0.016000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">454564Done </t>
+  </si>
+  <si>
+    <t>5000</t>
+  </si>
+  <si>
+    <t>1000011210179768581</t>
+  </si>
+  <si>
+    <t>Your transaction is successful</t>
+  </si>
+  <si>
+    <t>TC_LoginCardholderPortal</t>
+  </si>
+  <si>
+    <t>TC_viewChargeForRefundOnWalletClosure</t>
+  </si>
+  <si>
+    <t>10000173090000012</t>
+  </si>
+  <si>
+    <t>aBcd1234*</t>
+  </si>
+  <si>
+    <t>TC_masterCardMoneyTransfer</t>
+  </si>
+  <si>
+    <t>4564564564654654564</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>CMKO-45</t>
+  </si>
+  <si>
+    <t>TC_checkInterbankTransfer</t>
+  </si>
+  <si>
+    <t>TC_viewTransactionHistoryForWallet</t>
+  </si>
+  <si>
+    <t>05/10/2017</t>
+  </si>
+  <si>
+    <t>31/10/2017</t>
+  </si>
+  <si>
+    <t>TC_deviceReplaceService</t>
+  </si>
+  <si>
+    <t>Emergency Replacement</t>
+  </si>
+  <si>
+    <t>Request is forwarded to institution</t>
+  </si>
+  <si>
+    <t>TC_deviceBlockFromCardHolder</t>
+  </si>
+  <si>
+    <t>Card need to block as it is stolne</t>
+  </si>
+  <si>
+    <t>Device Blocked Call Reference Number</t>
+  </si>
+  <si>
+    <t>Block my card</t>
+  </si>
+  <si>
+    <t>Unblock Device process successful</t>
+  </si>
+  <si>
+    <t>TC_deviceUnblockFromCardholder</t>
+  </si>
+  <si>
+    <t>TC_walletActivateFromCardHolder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activate Wallet </t>
+  </si>
+  <si>
+    <t>Request has been processed successfully with reference number</t>
+  </si>
+  <si>
+    <t>TC_walletDeActivateFromCardHolder</t>
+  </si>
+  <si>
+    <t>Deactivate Wallet</t>
+  </si>
+  <si>
+    <t>TC_activateEcomForLifeLong</t>
+  </si>
+  <si>
+    <t>DEVICE is already activated for life long use</t>
+  </si>
+  <si>
+    <t>TC_activationEcomForDuration</t>
+  </si>
+  <si>
+    <t>TC_activateEcomForNHours</t>
+  </si>
+  <si>
+    <t>TC_cashRemittanceBookting</t>
+  </si>
+  <si>
+    <t>000000070</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>Fname</t>
+  </si>
+  <si>
+    <t>Mname</t>
+  </si>
+  <si>
+    <t>Lname</t>
+  </si>
+  <si>
+    <t>Address1</t>
+  </si>
+  <si>
+    <t>Address3</t>
+  </si>
+  <si>
+    <t>INDIA</t>
+  </si>
+  <si>
+    <t>MAHARASTHRA</t>
+  </si>
+  <si>
+    <t>mastercard@mastercard.com</t>
+  </si>
+  <si>
+    <t>INR</t>
+  </si>
+  <si>
+    <t>TC_signUpCardholderPortal</t>
+  </si>
+  <si>
+    <t>TC_activationForInternationalUse</t>
+  </si>
+  <si>
+    <t>TC_activationNHoursForInternationalUse</t>
+  </si>
+  <si>
+    <t>TC_activationLifeLongForInternationalUse</t>
   </si>
 </sst>
 </file>
@@ -1629,7 +1953,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1695,6 +2019,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2644,7 +2979,363 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:O9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.44140625" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
+    <col min="8" max="8" width="16.21875" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" customWidth="1"/>
+    <col min="11" max="15" width="17.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>351</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>349</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>350</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>476</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>477</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>271</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>270</v>
+      </c>
+      <c r="J1" s="30" t="s">
+        <v>272</v>
+      </c>
+      <c r="K1" s="30" t="s">
+        <v>273</v>
+      </c>
+      <c r="L1" s="30" t="s">
+        <v>478</v>
+      </c>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+    </row>
+    <row r="2" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="32" t="s">
+        <v>280</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>495</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>454</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>353</v>
+      </c>
+      <c r="E2" s="32">
+        <v>4656</v>
+      </c>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32" t="s">
+        <v>467</v>
+      </c>
+      <c r="H2" s="32" t="s">
+        <v>390</v>
+      </c>
+      <c r="I2" s="32" t="s">
+        <v>479</v>
+      </c>
+      <c r="J2" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+    </row>
+    <row r="3" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="32" t="s">
+        <v>480</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>495</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>454</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>353</v>
+      </c>
+      <c r="E3" s="32">
+        <v>4656</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>481</v>
+      </c>
+      <c r="G3" s="32" t="s">
+        <v>467</v>
+      </c>
+      <c r="H3" s="32" t="s">
+        <v>390</v>
+      </c>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="32"/>
+    </row>
+    <row r="4" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="32" t="s">
+        <v>482</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>495</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>454</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>353</v>
+      </c>
+      <c r="E4" s="32">
+        <v>4656</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>483</v>
+      </c>
+      <c r="G4" s="32" t="s">
+        <v>467</v>
+      </c>
+      <c r="H4" s="32" t="s">
+        <v>390</v>
+      </c>
+      <c r="I4" s="32" t="s">
+        <v>484</v>
+      </c>
+      <c r="J4" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="32"/>
+    </row>
+    <row r="5" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="32" t="s">
+        <v>485</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>495</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>454</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>353</v>
+      </c>
+      <c r="E5" s="32">
+        <v>4656</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>481</v>
+      </c>
+      <c r="G5" s="32" t="s">
+        <v>467</v>
+      </c>
+      <c r="H5" s="32" t="s">
+        <v>390</v>
+      </c>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="32"/>
+      <c r="O5" s="32"/>
+    </row>
+    <row r="6" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="32" t="s">
+        <v>486</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>495</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>454</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>353</v>
+      </c>
+      <c r="E6" s="32">
+        <v>4656</v>
+      </c>
+      <c r="F6" s="32" t="s">
+        <v>481</v>
+      </c>
+      <c r="G6" s="32" t="s">
+        <v>467</v>
+      </c>
+      <c r="H6" s="32" t="s">
+        <v>390</v>
+      </c>
+      <c r="I6" s="32" t="s">
+        <v>487</v>
+      </c>
+      <c r="J6" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="32"/>
+      <c r="O6" s="32"/>
+    </row>
+    <row r="7" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="32" t="s">
+        <v>488</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>495</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>454</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>353</v>
+      </c>
+      <c r="E7" s="32">
+        <v>4656</v>
+      </c>
+      <c r="F7" s="32" t="s">
+        <v>481</v>
+      </c>
+      <c r="G7" s="32" t="s">
+        <v>467</v>
+      </c>
+      <c r="H7" s="32" t="s">
+        <v>390</v>
+      </c>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32" t="s">
+        <v>489</v>
+      </c>
+      <c r="M7" s="32"/>
+      <c r="N7" s="32"/>
+      <c r="O7" s="32"/>
+    </row>
+    <row r="8" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="32" t="s">
+        <v>490</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>495</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>454</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>353</v>
+      </c>
+      <c r="E8" s="32">
+        <v>4656</v>
+      </c>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32" t="s">
+        <v>467</v>
+      </c>
+      <c r="H8" s="32" t="s">
+        <v>390</v>
+      </c>
+      <c r="I8" s="32" t="s">
+        <v>491</v>
+      </c>
+      <c r="J8" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="K8" s="32" t="s">
+        <v>492</v>
+      </c>
+      <c r="L8" s="32"/>
+      <c r="M8" s="32"/>
+      <c r="N8" s="32"/>
+      <c r="O8" s="32"/>
+    </row>
+    <row r="9" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="32" t="s">
+        <v>493</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>495</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>454</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>353</v>
+      </c>
+      <c r="E9" s="32">
+        <v>4656</v>
+      </c>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32" t="s">
+        <v>467</v>
+      </c>
+      <c r="H9" s="32" t="s">
+        <v>390</v>
+      </c>
+      <c r="I9" s="32" t="s">
+        <v>494</v>
+      </c>
+      <c r="J9" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="32"/>
+      <c r="O9" s="32"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
@@ -2664,7 +3355,7 @@
     <col min="11" max="11" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
         <v>1</v>
       </c>
@@ -2695,7 +3386,7 @@
       <c r="J1" s="30"/>
       <c r="K1" s="34"/>
     </row>
-    <row r="2" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>281</v>
       </c>
@@ -2724,7 +3415,7 @@
       <c r="J2" s="32"/>
       <c r="K2" s="32"/>
     </row>
-    <row r="3" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="32" t="s">
         <v>283</v>
       </c>
@@ -2753,7 +3444,7 @@
       <c r="J3" s="32"/>
       <c r="K3" s="32"/>
     </row>
-    <row r="4" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="32" t="s">
         <v>285</v>
       </c>
@@ -2782,23 +3473,14 @@
       <c r="J4" s="32"/>
       <c r="K4" s="32"/>
     </row>
-    <row r="5" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
@@ -2943,10 +3625,6 @@
         <v>303</v>
       </c>
     </row>
-    <row r="3" spans="1:19" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:19" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:19" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:19" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
@@ -2955,9 +3633,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
@@ -2977,7 +3655,7 @@
     <col min="11" max="11" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
         <v>1</v>
       </c>
@@ -3008,7 +3686,7 @@
       <c r="J1" s="30"/>
       <c r="K1" s="34"/>
     </row>
-    <row r="2" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>274</v>
       </c>
@@ -3039,7 +3717,7 @@
       <c r="J2" s="32"/>
       <c r="K2" s="32"/>
     </row>
-    <row r="3" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="32" t="s">
         <v>278</v>
       </c>
@@ -3070,22 +3748,12 @@
       <c r="J3" s="32"/>
       <c r="K3" s="32"/>
     </row>
-    <row r="4" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD2"/>
   <sheetViews>
@@ -3310,7 +3978,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S9"/>
   <sheetViews>
@@ -7286,7 +7954,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA23"/>
+  <dimension ref="A1:AA22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
@@ -7311,7 +7979,7 @@
     <col min="28" max="16384" width="8.88671875" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
         <v>1</v>
       </c>
@@ -7394,7 +8062,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="2" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>389</v>
       </c>
@@ -7449,7 +8117,7 @@
       <c r="Z2" s="32"/>
       <c r="AA2" s="32"/>
     </row>
-    <row r="3" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="32" t="s">
         <v>392</v>
       </c>
@@ -7494,7 +8162,7 @@
       <c r="Z3" s="32"/>
       <c r="AA3" s="32"/>
     </row>
-    <row r="4" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="32" t="s">
         <v>396</v>
       </c>
@@ -7539,7 +8207,7 @@
       <c r="Z4" s="32"/>
       <c r="AA4" s="32"/>
     </row>
-    <row r="5" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" s="32" t="s">
         <v>399</v>
       </c>
@@ -7584,7 +8252,7 @@
       <c r="Z5" s="32"/>
       <c r="AA5" s="32"/>
     </row>
-    <row r="6" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" s="32" t="s">
         <v>402</v>
       </c>
@@ -7629,7 +8297,7 @@
       <c r="Z6" s="32"/>
       <c r="AA6" s="32"/>
     </row>
-    <row r="7" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" s="32" t="s">
         <v>403</v>
       </c>
@@ -7674,7 +8342,7 @@
       <c r="Z7" s="32"/>
       <c r="AA7" s="32"/>
     </row>
-    <row r="8" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" s="32" t="s">
         <v>404</v>
       </c>
@@ -7715,7 +8383,7 @@
       <c r="Z8" s="32"/>
       <c r="AA8" s="32"/>
     </row>
-    <row r="9" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" s="32" t="s">
         <v>405</v>
       </c>
@@ -7756,7 +8424,7 @@
       <c r="Z9" s="32"/>
       <c r="AA9" s="32"/>
     </row>
-    <row r="10" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" s="32" t="s">
         <v>406</v>
       </c>
@@ -7797,7 +8465,7 @@
       <c r="Z10" s="32"/>
       <c r="AA10" s="32"/>
     </row>
-    <row r="11" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" s="32" t="s">
         <v>409</v>
       </c>
@@ -7840,7 +8508,7 @@
       <c r="Z11" s="32"/>
       <c r="AA11" s="32"/>
     </row>
-    <row r="12" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" s="32" t="s">
         <v>411</v>
       </c>
@@ -7883,7 +8551,7 @@
       <c r="Z12" s="32"/>
       <c r="AA12" s="32"/>
     </row>
-    <row r="13" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13" s="32" t="s">
         <v>413</v>
       </c>
@@ -7926,7 +8594,7 @@
       <c r="Z13" s="32"/>
       <c r="AA13" s="32"/>
     </row>
-    <row r="14" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" s="32" t="s">
         <v>415</v>
       </c>
@@ -7969,7 +8637,7 @@
       <c r="Z14" s="32"/>
       <c r="AA14" s="32"/>
     </row>
-    <row r="15" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" s="32" t="s">
         <v>417</v>
       </c>
@@ -8012,7 +8680,7 @@
       <c r="Z15" s="32"/>
       <c r="AA15" s="32"/>
     </row>
-    <row r="16" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16" s="32" t="s">
         <v>418</v>
       </c>
@@ -8055,7 +8723,7 @@
       <c r="Z16" s="32"/>
       <c r="AA16" s="32"/>
     </row>
-    <row r="17" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17" s="32" t="s">
         <v>420</v>
       </c>
@@ -8116,7 +8784,7 @@
       </c>
       <c r="AA17" s="32"/>
     </row>
-    <row r="18" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18" s="32" t="s">
         <v>426</v>
       </c>
@@ -8171,7 +8839,7 @@
       </c>
       <c r="AA18" s="32"/>
     </row>
-    <row r="19" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19" s="32" t="s">
         <v>430</v>
       </c>
@@ -8228,7 +8896,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="20" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A20" s="32" t="s">
         <v>433</v>
       </c>
@@ -8285,7 +8953,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="21" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A21" s="32" t="s">
         <v>435</v>
       </c>
@@ -8342,7 +9010,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="22" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A22" s="32" t="s">
         <v>437</v>
       </c>
@@ -8399,7 +9067,6 @@
         <v>432</v>
       </c>
     </row>
-    <row r="23" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8407,7 +9074,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q23"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
@@ -8431,7 +9098,7 @@
     <col min="18" max="16384" width="8.88671875" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
         <v>1</v>
       </c>
@@ -8474,8 +9141,11 @@
       <c r="N1" s="30" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>447</v>
       </c>
@@ -8514,99 +9184,24 @@
       <c r="N2" s="32" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O5"/>
-      <c r="P5"/>
-      <c r="Q5"/>
-    </row>
-    <row r="6" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O6"/>
-      <c r="P6"/>
-      <c r="Q6"/>
-    </row>
-    <row r="7" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O7"/>
-      <c r="P7"/>
-      <c r="Q7"/>
-    </row>
-    <row r="8" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O8"/>
-      <c r="P8"/>
-      <c r="Q8"/>
-    </row>
-    <row r="9" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O9"/>
-      <c r="P9"/>
-      <c r="Q9"/>
-    </row>
-    <row r="10" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O10"/>
-      <c r="P10"/>
-      <c r="Q10"/>
-    </row>
-    <row r="11" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O11"/>
-      <c r="P11"/>
-      <c r="Q11"/>
-    </row>
-    <row r="12" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O12"/>
-      <c r="P12"/>
-      <c r="Q12"/>
-    </row>
-    <row r="13" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O14"/>
-      <c r="P14"/>
-      <c r="Q14"/>
-    </row>
-    <row r="15" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O15"/>
-      <c r="P15"/>
-      <c r="Q15"/>
-    </row>
-    <row r="16" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O16"/>
-      <c r="P16"/>
-      <c r="Q16"/>
-    </row>
-    <row r="17" spans="15:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O17"/>
-      <c r="P17"/>
-      <c r="Q17"/>
-    </row>
-    <row r="18" spans="15:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O18"/>
-      <c r="P18"/>
-      <c r="Q18"/>
-    </row>
-    <row r="19" spans="15:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O19"/>
-      <c r="P19"/>
-      <c r="Q19"/>
-    </row>
-    <row r="20" spans="15:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O20"/>
-      <c r="P20"/>
-      <c r="Q20"/>
-    </row>
-    <row r="21" spans="15:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O21"/>
-      <c r="P21"/>
-      <c r="Q21"/>
-    </row>
-    <row r="22" spans="15:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O22"/>
-      <c r="P22"/>
-      <c r="Q22"/>
-    </row>
-    <row r="23" spans="15:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O23"/>
-      <c r="P23"/>
-      <c r="Q23"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="31"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="31"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O13" s="31"/>
+      <c r="P13" s="31"/>
+      <c r="Q13" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8615,9 +9210,9 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -8634,7 +9229,7 @@
     <col min="11" max="11" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
         <v>1</v>
       </c>
@@ -8669,7 +9264,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>459</v>
       </c>
@@ -8702,17 +9297,6 @@
         <v>462</v>
       </c>
     </row>
-    <row r="3" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please select from the dropdown" sqref="J2">
@@ -8725,7 +9309,2023 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:BC20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="40.5546875" customWidth="1"/>
+    <col min="2" max="2" width="49.88671875" customWidth="1"/>
+    <col min="3" max="3" width="24.21875" style="42" customWidth="1"/>
+    <col min="4" max="4" width="19.109375" style="43" customWidth="1"/>
+    <col min="5" max="5" width="18.5546875" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" customWidth="1"/>
+    <col min="7" max="7" width="18.88671875" customWidth="1"/>
+    <col min="8" max="8" width="13.77734375" style="43" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" style="43" customWidth="1"/>
+    <col min="10" max="10" width="18.109375" style="43" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" customWidth="1"/>
+    <col min="12" max="12" width="15.44140625" customWidth="1"/>
+    <col min="13" max="13" width="14.77734375" customWidth="1"/>
+    <col min="15" max="15" width="19.6640625" customWidth="1"/>
+    <col min="16" max="16" width="18.21875" customWidth="1"/>
+    <col min="17" max="17" width="30.88671875" customWidth="1"/>
+    <col min="18" max="18" width="22.33203125" customWidth="1"/>
+    <col min="19" max="19" width="30.44140625" customWidth="1"/>
+    <col min="20" max="20" width="31.88671875" customWidth="1"/>
+    <col min="21" max="21" width="23.109375" customWidth="1"/>
+    <col min="22" max="22" width="12.21875" style="43" customWidth="1"/>
+    <col min="23" max="23" width="12.44140625" customWidth="1"/>
+    <col min="24" max="24" width="24.33203125" customWidth="1"/>
+    <col min="25" max="25" width="31.5546875" customWidth="1"/>
+    <col min="26" max="26" width="33.5546875" customWidth="1"/>
+    <col min="27" max="27" width="29.77734375" customWidth="1"/>
+    <col min="28" max="28" width="28" customWidth="1"/>
+    <col min="29" max="29" width="30.5546875" customWidth="1"/>
+    <col min="30" max="30" width="24.6640625" customWidth="1"/>
+    <col min="31" max="31" width="22.88671875" customWidth="1"/>
+    <col min="32" max="32" width="45.21875" customWidth="1"/>
+    <col min="33" max="33" width="56.6640625" customWidth="1"/>
+    <col min="34" max="34" width="41.109375" customWidth="1"/>
+    <col min="35" max="35" width="16.5546875" customWidth="1"/>
+    <col min="36" max="36" width="19.6640625" customWidth="1"/>
+    <col min="37" max="37" width="22.88671875" customWidth="1"/>
+    <col min="38" max="38" width="18.44140625" customWidth="1"/>
+    <col min="39" max="40" width="22.33203125" customWidth="1"/>
+    <col min="41" max="42" width="22.5546875" customWidth="1"/>
+    <col min="43" max="43" width="24.44140625" customWidth="1"/>
+    <col min="44" max="44" width="20.109375" customWidth="1"/>
+    <col min="45" max="45" width="19.109375" customWidth="1"/>
+    <col min="46" max="46" width="23.6640625" customWidth="1"/>
+    <col min="47" max="47" width="23.5546875" customWidth="1"/>
+    <col min="48" max="48" width="29.6640625" customWidth="1"/>
+    <col min="49" max="49" width="28.88671875" customWidth="1"/>
+    <col min="50" max="55" width="24.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A1" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>351</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>349</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>350</v>
+      </c>
+      <c r="E1" s="35" t="s">
+        <v>497</v>
+      </c>
+      <c r="F1" s="35" t="s">
+        <v>498</v>
+      </c>
+      <c r="G1" s="35" t="s">
+        <v>499</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>500</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>501</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>502</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>503</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>504</v>
+      </c>
+      <c r="M1" s="20" t="s">
+        <v>505</v>
+      </c>
+      <c r="N1" s="20" t="s">
+        <v>506</v>
+      </c>
+      <c r="O1" s="20" t="s">
+        <v>507</v>
+      </c>
+      <c r="P1" s="20" t="s">
+        <v>508</v>
+      </c>
+      <c r="Q1" s="20" t="s">
+        <v>509</v>
+      </c>
+      <c r="R1" s="20" t="s">
+        <v>510</v>
+      </c>
+      <c r="S1" s="37" t="s">
+        <v>511</v>
+      </c>
+      <c r="T1" s="21" t="s">
+        <v>512</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="Z1" s="20" t="s">
+        <v>518</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="AJ1" s="38" t="s">
+        <v>528</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="2" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F2" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" t="s">
+        <v>551</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="Q2" s="24" t="s">
+        <v>556</v>
+      </c>
+      <c r="R2" s="24" t="s">
+        <v>553</v>
+      </c>
+      <c r="S2" s="24" t="s">
+        <v>557</v>
+      </c>
+      <c r="T2" s="40" t="s">
+        <v>558</v>
+      </c>
+      <c r="U2" s="2"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
+      <c r="AG2" s="2"/>
+      <c r="AH2" s="2"/>
+      <c r="AI2" s="2"/>
+      <c r="AJ2" s="2"/>
+      <c r="AK2" s="2"/>
+      <c r="AL2" s="2"/>
+      <c r="AM2" s="2"/>
+      <c r="AN2" s="2"/>
+      <c r="AO2" s="2"/>
+      <c r="AP2" s="2"/>
+      <c r="AQ2" s="2"/>
+      <c r="AR2" s="2"/>
+      <c r="AS2" s="2"/>
+      <c r="AT2" s="2"/>
+      <c r="AU2" s="2"/>
+      <c r="AV2" s="2"/>
+      <c r="AW2" s="2"/>
+      <c r="AX2" s="2"/>
+      <c r="AY2" s="2"/>
+      <c r="AZ2" s="2"/>
+      <c r="BA2" s="2"/>
+      <c r="BB2" s="2"/>
+      <c r="BC2" s="2"/>
+    </row>
+    <row r="3" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F3" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="2"/>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2"/>
+      <c r="AJ3" s="2"/>
+      <c r="AK3" s="2"/>
+      <c r="AL3" s="2"/>
+      <c r="AM3" s="2"/>
+      <c r="AN3" s="2"/>
+      <c r="AO3" s="2"/>
+      <c r="AP3" s="2"/>
+      <c r="AQ3" s="2"/>
+      <c r="AR3" s="2"/>
+      <c r="AS3" s="2"/>
+      <c r="AT3" s="2"/>
+      <c r="AU3" s="2"/>
+      <c r="AV3" s="2"/>
+      <c r="AW3" s="2"/>
+      <c r="AX3" s="2"/>
+      <c r="AY3" s="2"/>
+      <c r="AZ3" s="2"/>
+      <c r="BA3" s="2"/>
+      <c r="BB3" s="2"/>
+      <c r="BC3" s="2"/>
+    </row>
+    <row r="4" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="B4" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>561</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>562</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F4" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
+      <c r="AF4" s="2"/>
+      <c r="AG4" s="2"/>
+      <c r="AH4" s="2"/>
+      <c r="AI4" s="2"/>
+      <c r="AJ4" s="2"/>
+      <c r="AK4" s="2"/>
+      <c r="AL4" s="2"/>
+      <c r="AM4" s="2"/>
+      <c r="AN4" s="2"/>
+      <c r="AO4" s="2"/>
+      <c r="AP4" s="2"/>
+      <c r="AQ4" s="2"/>
+      <c r="AR4" s="2"/>
+      <c r="AS4" s="2"/>
+      <c r="AT4" s="2"/>
+      <c r="AU4" s="2"/>
+      <c r="AV4" s="2"/>
+      <c r="AW4" s="2"/>
+      <c r="AX4" s="2"/>
+      <c r="AY4" s="2"/>
+      <c r="AZ4" s="2"/>
+      <c r="BA4" s="2"/>
+      <c r="BB4" s="2"/>
+      <c r="BC4" s="2"/>
+    </row>
+    <row r="5" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F5" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>564</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>556</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="L5" s="2">
+        <v>955689456</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="O5" t="s">
+        <v>551</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="9"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="2"/>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="2"/>
+      <c r="AF5" s="2"/>
+      <c r="AG5" s="2"/>
+      <c r="AH5" s="2"/>
+      <c r="AI5" s="2"/>
+      <c r="AJ5" s="2"/>
+      <c r="AK5" s="2"/>
+      <c r="AL5" s="2"/>
+      <c r="AM5" s="2"/>
+      <c r="AN5" s="2"/>
+      <c r="AO5" s="2"/>
+      <c r="AP5" s="2"/>
+      <c r="AQ5" s="2"/>
+      <c r="AR5" s="2"/>
+      <c r="AS5" s="2"/>
+      <c r="AT5" s="2"/>
+      <c r="AU5" s="2"/>
+      <c r="AV5" s="2"/>
+      <c r="AW5" s="2"/>
+      <c r="AX5" s="2"/>
+      <c r="AY5" s="2"/>
+      <c r="AZ5" s="2"/>
+      <c r="BA5" s="2"/>
+      <c r="BB5" s="2"/>
+      <c r="BC5" s="2"/>
+    </row>
+    <row r="6" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="B6" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F6" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="2"/>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="2"/>
+      <c r="AF6" s="2"/>
+      <c r="AG6" s="2"/>
+      <c r="AH6" s="2"/>
+      <c r="AI6" s="2"/>
+      <c r="AJ6" s="2"/>
+      <c r="AK6" s="2"/>
+      <c r="AL6" s="2"/>
+      <c r="AM6" s="2"/>
+      <c r="AN6" s="2"/>
+      <c r="AO6" s="2"/>
+      <c r="AP6" s="2"/>
+      <c r="AQ6" s="2"/>
+      <c r="AR6" s="2"/>
+      <c r="AS6" s="2"/>
+      <c r="AT6" s="2"/>
+      <c r="AU6" s="2"/>
+      <c r="AV6" s="2"/>
+      <c r="AW6" s="2"/>
+      <c r="AX6" s="2"/>
+      <c r="AY6" s="2"/>
+      <c r="AZ6" s="2"/>
+      <c r="BA6" s="2"/>
+      <c r="BB6" s="2"/>
+      <c r="BC6" s="2"/>
+    </row>
+    <row r="7" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="B7" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F7" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2">
+        <v>10</v>
+      </c>
+      <c r="V7" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="2"/>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="2"/>
+      <c r="AE7" s="2"/>
+      <c r="AF7" s="2"/>
+      <c r="AG7" s="2"/>
+      <c r="AH7" s="2"/>
+      <c r="AI7" s="2"/>
+      <c r="AJ7" s="2"/>
+      <c r="AK7" s="2"/>
+      <c r="AL7" s="2"/>
+      <c r="AM7" s="2"/>
+      <c r="AN7" s="2"/>
+      <c r="AO7" s="2"/>
+      <c r="AP7" s="2"/>
+      <c r="AQ7" s="2"/>
+      <c r="AR7" s="2"/>
+      <c r="AS7" s="2"/>
+      <c r="AT7" s="2"/>
+      <c r="AU7" s="2"/>
+      <c r="AV7" s="2"/>
+      <c r="AW7" s="2"/>
+      <c r="AX7" s="2"/>
+      <c r="AY7" s="2"/>
+      <c r="AZ7" s="2"/>
+      <c r="BA7" s="2"/>
+      <c r="BB7" s="2"/>
+      <c r="BC7" s="2"/>
+    </row>
+    <row r="8" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F8" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2">
+        <v>10</v>
+      </c>
+      <c r="V8" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="W8" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="X8" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="Y8" s="40" t="s">
+        <v>573</v>
+      </c>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2"/>
+      <c r="AD8" s="2"/>
+      <c r="AE8" s="2"/>
+      <c r="AF8" s="2"/>
+      <c r="AG8" s="2"/>
+      <c r="AH8" s="2"/>
+      <c r="AI8" s="2"/>
+      <c r="AJ8" s="2"/>
+      <c r="AK8" s="2"/>
+      <c r="AL8" s="2"/>
+      <c r="AM8" s="2"/>
+      <c r="AN8" s="2"/>
+      <c r="AO8" s="2"/>
+      <c r="AP8" s="2"/>
+      <c r="AQ8" s="2"/>
+      <c r="AR8" s="2"/>
+      <c r="AS8" s="2"/>
+      <c r="AT8" s="2"/>
+      <c r="AU8" s="2"/>
+      <c r="AV8" s="2"/>
+      <c r="AW8" s="2"/>
+      <c r="AX8" s="2"/>
+      <c r="AY8" s="2"/>
+      <c r="AZ8" s="2"/>
+      <c r="BA8" s="2"/>
+      <c r="BB8" s="2"/>
+      <c r="BC8" s="2"/>
+    </row>
+    <row r="9" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="B9" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F9" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2">
+        <v>10</v>
+      </c>
+      <c r="V9" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="W9" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="X9" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="Y9" s="40" t="s">
+        <v>573</v>
+      </c>
+      <c r="Z9" s="40" t="s">
+        <v>575</v>
+      </c>
+      <c r="AA9" s="40" t="s">
+        <v>576</v>
+      </c>
+      <c r="AB9" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="AC9" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="AD9" s="2"/>
+      <c r="AE9" s="2"/>
+      <c r="AF9" s="2"/>
+      <c r="AG9" s="2"/>
+      <c r="AH9" s="2"/>
+      <c r="AI9" s="2"/>
+      <c r="AJ9" s="2"/>
+      <c r="AK9" s="2"/>
+      <c r="AL9" s="2"/>
+      <c r="AM9" s="2"/>
+      <c r="AN9" s="2"/>
+      <c r="AO9" s="2"/>
+      <c r="AP9" s="2"/>
+      <c r="AQ9" s="2"/>
+      <c r="AR9" s="2"/>
+      <c r="AS9" s="2"/>
+      <c r="AT9" s="2"/>
+      <c r="AU9" s="2"/>
+      <c r="AV9" s="2"/>
+      <c r="AW9" s="2"/>
+      <c r="AX9" s="2"/>
+      <c r="AY9" s="2"/>
+      <c r="AZ9" s="2"/>
+      <c r="BA9" s="2"/>
+      <c r="BB9" s="2"/>
+      <c r="BC9" s="2"/>
+    </row>
+    <row r="10" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="B10" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F10" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2">
+        <v>10</v>
+      </c>
+      <c r="V10" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="W10" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="X10" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="Y10" s="40" t="s">
+        <v>573</v>
+      </c>
+      <c r="Z10" s="40" t="s">
+        <v>575</v>
+      </c>
+      <c r="AA10" s="40" t="s">
+        <v>576</v>
+      </c>
+      <c r="AB10" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="AC10" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="AD10" s="2"/>
+      <c r="AE10" s="2"/>
+      <c r="AF10" s="2"/>
+      <c r="AG10" s="2"/>
+      <c r="AH10" s="2"/>
+      <c r="AI10" s="2"/>
+      <c r="AJ10" s="2"/>
+      <c r="AK10" s="2"/>
+      <c r="AL10" s="2"/>
+      <c r="AM10" s="2"/>
+      <c r="AN10" s="2"/>
+      <c r="AO10" s="2"/>
+      <c r="AP10" s="2"/>
+      <c r="AQ10" s="2"/>
+      <c r="AR10" s="2"/>
+      <c r="AS10" s="2"/>
+      <c r="AT10" s="2"/>
+      <c r="AU10" s="2"/>
+      <c r="AV10" s="2"/>
+      <c r="AW10" s="2"/>
+      <c r="AX10" s="2"/>
+      <c r="AY10" s="2"/>
+      <c r="AZ10" s="2"/>
+      <c r="BA10" s="2"/>
+      <c r="BB10" s="2"/>
+      <c r="BC10" s="2"/>
+    </row>
+    <row r="11" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="B11" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F11" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2">
+        <v>10</v>
+      </c>
+      <c r="V11" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="W11" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="X11" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="Y11" s="40" t="s">
+        <v>573</v>
+      </c>
+      <c r="Z11" s="40" t="s">
+        <v>575</v>
+      </c>
+      <c r="AA11" s="40" t="s">
+        <v>576</v>
+      </c>
+      <c r="AB11" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="AC11" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="AD11" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="AE11" s="2"/>
+      <c r="AF11" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="AG11" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="AH11" s="2"/>
+      <c r="AI11" s="2"/>
+      <c r="AJ11" s="2"/>
+      <c r="AK11" s="2"/>
+      <c r="AL11" s="2"/>
+      <c r="AM11" s="2"/>
+      <c r="AN11" s="2"/>
+      <c r="AO11" s="2"/>
+      <c r="AP11" s="2"/>
+      <c r="AQ11" s="2"/>
+      <c r="AR11" s="2"/>
+      <c r="AS11" s="2"/>
+      <c r="AT11" s="2"/>
+      <c r="AU11" s="2"/>
+      <c r="AV11" s="2"/>
+      <c r="AW11" s="2"/>
+      <c r="AX11" s="2"/>
+      <c r="AY11" s="2"/>
+      <c r="AZ11" s="2"/>
+      <c r="BA11" s="2"/>
+      <c r="BB11" s="2"/>
+      <c r="BC11" s="2"/>
+    </row>
+    <row r="12" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="B12" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F12" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2">
+        <v>10</v>
+      </c>
+      <c r="V12" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="W12" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="X12" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="Y12" s="40" t="s">
+        <v>573</v>
+      </c>
+      <c r="Z12" s="40" t="s">
+        <v>575</v>
+      </c>
+      <c r="AA12" s="40" t="s">
+        <v>576</v>
+      </c>
+      <c r="AB12" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="AC12" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="AD12" s="2"/>
+      <c r="AE12" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="AF12" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="AG12" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="AH12" s="2"/>
+      <c r="AI12" s="2"/>
+      <c r="AJ12" s="2"/>
+      <c r="AK12" s="2"/>
+      <c r="AL12" s="2"/>
+      <c r="AM12" s="2"/>
+      <c r="AN12" s="2"/>
+      <c r="AO12" s="2"/>
+      <c r="AP12" s="2"/>
+      <c r="AQ12" s="2"/>
+      <c r="AR12" s="2"/>
+      <c r="AS12" s="2"/>
+      <c r="AT12" s="2"/>
+      <c r="AU12" s="2"/>
+      <c r="AV12" s="2"/>
+      <c r="AW12" s="2"/>
+      <c r="AX12" s="2"/>
+      <c r="AY12" s="2"/>
+      <c r="AZ12" s="2"/>
+      <c r="BA12" s="2"/>
+      <c r="BB12" s="2"/>
+      <c r="BC12" s="2"/>
+    </row>
+    <row r="13" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="B13" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F13" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2">
+        <v>10</v>
+      </c>
+      <c r="V13" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="W13" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="X13" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="Y13" s="40" t="s">
+        <v>573</v>
+      </c>
+      <c r="Z13" s="40" t="s">
+        <v>575</v>
+      </c>
+      <c r="AA13" s="40" t="s">
+        <v>576</v>
+      </c>
+      <c r="AB13" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="AC13" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="AD13" s="2"/>
+      <c r="AE13" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="AF13" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="AG13" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="AH13" s="40" t="s">
+        <v>586</v>
+      </c>
+      <c r="AI13" s="2"/>
+      <c r="AJ13" s="2"/>
+      <c r="AK13" s="2"/>
+      <c r="AL13" s="2"/>
+      <c r="AM13" s="2"/>
+      <c r="AN13" s="2"/>
+      <c r="AO13" s="2"/>
+      <c r="AP13" s="2"/>
+      <c r="AQ13" s="2"/>
+      <c r="AR13" s="2"/>
+      <c r="AS13" s="2"/>
+      <c r="AT13" s="2"/>
+      <c r="AU13" s="2"/>
+      <c r="AV13" s="2"/>
+      <c r="AW13" s="2"/>
+      <c r="AX13" s="2"/>
+      <c r="AY13" s="2"/>
+      <c r="AZ13" s="2"/>
+      <c r="BA13" s="2"/>
+      <c r="BB13" s="2"/>
+      <c r="BC13" s="2"/>
+    </row>
+    <row r="14" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="B14" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F14" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2">
+        <v>10</v>
+      </c>
+      <c r="V14" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="W14" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="X14" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="Y14" s="40" t="s">
+        <v>573</v>
+      </c>
+      <c r="Z14" s="40" t="s">
+        <v>575</v>
+      </c>
+      <c r="AA14" s="40" t="s">
+        <v>576</v>
+      </c>
+      <c r="AB14" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="AC14" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="AD14" s="2"/>
+      <c r="AE14" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="AF14" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="AG14" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="AH14" s="40" t="s">
+        <v>586</v>
+      </c>
+      <c r="AI14" s="2"/>
+      <c r="AJ14" s="2"/>
+      <c r="AK14" s="2"/>
+      <c r="AL14" s="2"/>
+      <c r="AM14" s="2"/>
+      <c r="AN14" s="2"/>
+      <c r="AO14" s="2"/>
+      <c r="AP14" s="2"/>
+      <c r="AQ14" s="2"/>
+      <c r="AR14" s="2"/>
+      <c r="AS14" s="2"/>
+      <c r="AT14" s="2"/>
+      <c r="AU14" s="2"/>
+      <c r="AV14" s="2"/>
+      <c r="AW14" s="2"/>
+      <c r="AX14" s="2"/>
+      <c r="AY14" s="2"/>
+      <c r="AZ14" s="2"/>
+      <c r="BA14" s="2"/>
+      <c r="BB14" s="2"/>
+      <c r="BC14" s="2"/>
+    </row>
+    <row r="15" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="B15" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F15" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2">
+        <v>10</v>
+      </c>
+      <c r="V15" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="W15" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="X15" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="Y15" s="40" t="s">
+        <v>573</v>
+      </c>
+      <c r="Z15" s="40" t="s">
+        <v>575</v>
+      </c>
+      <c r="AA15" s="40" t="s">
+        <v>576</v>
+      </c>
+      <c r="AB15" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="AC15" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="AD15" s="2"/>
+      <c r="AE15" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="AF15" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="AG15" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="AH15" s="40" t="s">
+        <v>586</v>
+      </c>
+      <c r="AI15" s="2"/>
+      <c r="AJ15" s="2"/>
+      <c r="AK15" s="2"/>
+      <c r="AL15" s="2"/>
+      <c r="AM15" s="2"/>
+      <c r="AN15" s="2"/>
+      <c r="AO15" s="2"/>
+      <c r="AP15" s="2"/>
+      <c r="AQ15" s="2"/>
+      <c r="AR15" s="2"/>
+      <c r="AS15" s="2"/>
+      <c r="AT15" s="2"/>
+      <c r="AU15" s="2"/>
+      <c r="AV15" s="2"/>
+      <c r="AW15" s="2"/>
+      <c r="AX15" s="2"/>
+      <c r="AY15" s="2"/>
+      <c r="AZ15" s="2"/>
+      <c r="BA15" s="2"/>
+      <c r="BB15" s="2"/>
+      <c r="BC15" s="2"/>
+    </row>
+    <row r="16" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>589</v>
+      </c>
+      <c r="B16" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>561</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>590</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F16" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="9"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="2"/>
+      <c r="AB16" s="2"/>
+      <c r="AC16" s="2"/>
+      <c r="AD16" s="2"/>
+      <c r="AE16" s="2"/>
+      <c r="AF16" s="2"/>
+      <c r="AG16" s="2"/>
+      <c r="AH16" s="2"/>
+      <c r="AI16" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="AJ16" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="AK16" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="AL16" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="AM16" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="AN16" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="AO16" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="AP16" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="AQ16" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="AR16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AS16" s="2">
+        <v>411033</v>
+      </c>
+      <c r="AT16" s="41" t="s">
+        <v>599</v>
+      </c>
+      <c r="AU16" s="2">
+        <v>7896543215</v>
+      </c>
+      <c r="AV16" s="2">
+        <v>5000</v>
+      </c>
+      <c r="AW16" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="AX16" s="2"/>
+      <c r="AY16" s="2"/>
+      <c r="AZ16" s="2"/>
+      <c r="BA16" s="2"/>
+      <c r="BB16" s="2"/>
+      <c r="BC16" s="2"/>
+    </row>
+    <row r="17" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="B17" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F17" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="9"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2"/>
+      <c r="Y17" s="2"/>
+      <c r="Z17" s="2"/>
+      <c r="AA17" s="2"/>
+      <c r="AB17" s="2"/>
+      <c r="AC17" s="2"/>
+      <c r="AD17" s="2"/>
+      <c r="AE17" s="2"/>
+      <c r="AF17" s="2"/>
+      <c r="AG17" s="2"/>
+      <c r="AH17" s="2"/>
+      <c r="AI17" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="AJ17" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="AK17" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="AL17" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="AM17" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="AN17" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="AO17" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="AP17" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="AQ17" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="AR17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AS17" s="2">
+        <v>411033</v>
+      </c>
+      <c r="AT17" s="41" t="s">
+        <v>599</v>
+      </c>
+      <c r="AU17" s="2">
+        <v>7896543215</v>
+      </c>
+      <c r="AV17" s="2">
+        <v>5000</v>
+      </c>
+      <c r="AW17" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="AX17" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="AY17" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="AZ17" s="2"/>
+      <c r="BA17" s="2"/>
+      <c r="BB17" s="2"/>
+      <c r="BC17" s="2"/>
+    </row>
+    <row r="18" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="B18" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F18" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="9"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="2"/>
+      <c r="Z18" s="2"/>
+      <c r="AA18" s="2"/>
+      <c r="AB18" s="2"/>
+      <c r="AC18" s="2"/>
+      <c r="AD18" s="2"/>
+      <c r="AE18" s="2"/>
+      <c r="AF18" s="2"/>
+      <c r="AG18" s="2"/>
+      <c r="AH18" s="2"/>
+      <c r="AI18" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="AJ18" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="AK18" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="AL18" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="AM18" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="AN18" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="AO18" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="AP18" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="AQ18" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="AR18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AS18" s="2">
+        <v>411033</v>
+      </c>
+      <c r="AT18" s="41" t="s">
+        <v>599</v>
+      </c>
+      <c r="AU18" s="2">
+        <v>7896543215</v>
+      </c>
+      <c r="AV18" s="2">
+        <v>5000</v>
+      </c>
+      <c r="AW18" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="AX18" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="AY18" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="AZ18" s="2"/>
+      <c r="BA18" s="2"/>
+      <c r="BB18" s="2"/>
+      <c r="BC18" s="2"/>
+    </row>
+    <row r="19" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="B19" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F19" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="2"/>
+      <c r="Y19" s="2"/>
+      <c r="Z19" s="2"/>
+      <c r="AA19" s="2"/>
+      <c r="AB19" s="2"/>
+      <c r="AC19" s="2"/>
+      <c r="AD19" s="2"/>
+      <c r="AE19" s="2"/>
+      <c r="AF19" s="2"/>
+      <c r="AG19" s="2"/>
+      <c r="AH19" s="2"/>
+      <c r="AI19" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="AJ19" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="AK19" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="AL19" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="AM19" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="AN19" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="AO19" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="AP19" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="AQ19" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="AR19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AS19" s="2">
+        <v>411033</v>
+      </c>
+      <c r="AT19" s="41" t="s">
+        <v>599</v>
+      </c>
+      <c r="AU19" s="2">
+        <v>7896543215</v>
+      </c>
+      <c r="AV19" s="2">
+        <v>5000</v>
+      </c>
+      <c r="AW19" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="AX19" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="AY19" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="AZ19" s="2"/>
+      <c r="BA19" s="2"/>
+      <c r="BB19" s="2"/>
+      <c r="BC19" s="2"/>
+    </row>
+    <row r="20" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="B20" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F20" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
+      <c r="V20" s="9"/>
+      <c r="W20" s="2"/>
+      <c r="X20" s="2"/>
+      <c r="Y20" s="2"/>
+      <c r="Z20" s="2"/>
+      <c r="AA20" s="2"/>
+      <c r="AB20" s="2"/>
+      <c r="AC20" s="2"/>
+      <c r="AD20" s="2"/>
+      <c r="AE20" s="2"/>
+      <c r="AF20" s="2"/>
+      <c r="AG20" s="2"/>
+      <c r="AH20" s="2"/>
+      <c r="AI20" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="AJ20" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="AK20" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="AL20" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="AM20" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="AN20" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="AO20" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="AP20" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="AQ20" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="AR20" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AS20" s="2">
+        <v>411033</v>
+      </c>
+      <c r="AT20" s="41" t="s">
+        <v>599</v>
+      </c>
+      <c r="AU20" s="2">
+        <v>7896543215</v>
+      </c>
+      <c r="AV20" s="2">
+        <v>5000</v>
+      </c>
+      <c r="AW20" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="AX20" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="AY20" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="AZ20" s="2"/>
+      <c r="BA20" s="2"/>
+      <c r="BB20" s="2"/>
+      <c r="BC20" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2"/>
+    <hyperlink ref="B5" r:id="rId3"/>
+    <hyperlink ref="B16" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B2" r:id="rId6"/>
+    <hyperlink ref="B7" r:id="rId7"/>
+    <hyperlink ref="B8" r:id="rId8"/>
+    <hyperlink ref="B9" r:id="rId9"/>
+    <hyperlink ref="B10" r:id="rId10"/>
+    <hyperlink ref="B11" r:id="rId11"/>
+    <hyperlink ref="B12" r:id="rId12"/>
+    <hyperlink ref="B13" r:id="rId13"/>
+    <hyperlink ref="B14" r:id="rId14"/>
+    <hyperlink ref="B15" r:id="rId15"/>
+    <hyperlink ref="AT16" r:id="rId16"/>
+    <hyperlink ref="B17" r:id="rId17"/>
+    <hyperlink ref="AT17" r:id="rId18"/>
+    <hyperlink ref="B18" r:id="rId19"/>
+    <hyperlink ref="AT18" r:id="rId20"/>
+    <hyperlink ref="B19" r:id="rId21"/>
+    <hyperlink ref="AT19" r:id="rId22"/>
+    <hyperlink ref="B20" r:id="rId23"/>
+    <hyperlink ref="AT20" r:id="rId24"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
@@ -8744,7 +11344,7 @@
     <col min="11" max="15" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
         <v>1</v>
       </c>
@@ -8791,7 +11391,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>465</v>
       </c>
@@ -8834,7 +11434,7 @@
       </c>
       <c r="O2" s="32"/>
     </row>
-    <row r="3" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="32" t="s">
         <v>468</v>
       </c>
@@ -8877,7 +11477,7 @@
       </c>
       <c r="O3" s="32"/>
     </row>
-    <row r="4" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="32" t="s">
         <v>470</v>
       </c>
@@ -8922,7 +11522,7 @@
       </c>
       <c r="O4" s="32"/>
     </row>
-    <row r="5" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="32" t="s">
         <v>472</v>
       </c>
@@ -8965,7 +11565,7 @@
       </c>
       <c r="O5" s="32"/>
     </row>
-    <row r="6" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="32" t="s">
         <v>473</v>
       </c>
@@ -9010,373 +11610,6 @@
         <v>474</v>
       </c>
     </row>
-    <row r="7" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18.44140625" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" customWidth="1"/>
-    <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="16.21875" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" customWidth="1"/>
-    <col min="10" max="10" width="10.109375" customWidth="1"/>
-    <col min="11" max="15" width="17.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="30" t="s">
-        <v>351</v>
-      </c>
-      <c r="D1" s="30" t="s">
-        <v>349</v>
-      </c>
-      <c r="E1" s="30" t="s">
-        <v>350</v>
-      </c>
-      <c r="F1" s="30" t="s">
-        <v>476</v>
-      </c>
-      <c r="G1" s="30" t="s">
-        <v>477</v>
-      </c>
-      <c r="H1" s="30" t="s">
-        <v>271</v>
-      </c>
-      <c r="I1" s="30" t="s">
-        <v>270</v>
-      </c>
-      <c r="J1" s="30" t="s">
-        <v>272</v>
-      </c>
-      <c r="K1" s="30" t="s">
-        <v>273</v>
-      </c>
-      <c r="L1" s="30" t="s">
-        <v>478</v>
-      </c>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-    </row>
-    <row r="2" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="32" t="s">
-        <v>280</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>495</v>
-      </c>
-      <c r="C2" s="32" t="s">
-        <v>454</v>
-      </c>
-      <c r="D2" s="32" t="s">
-        <v>353</v>
-      </c>
-      <c r="E2" s="32">
-        <v>4656</v>
-      </c>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32" t="s">
-        <v>467</v>
-      </c>
-      <c r="H2" s="32" t="s">
-        <v>390</v>
-      </c>
-      <c r="I2" s="32" t="s">
-        <v>479</v>
-      </c>
-      <c r="J2" s="32" t="s">
-        <v>276</v>
-      </c>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-    </row>
-    <row r="3" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="32" t="s">
-        <v>480</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>495</v>
-      </c>
-      <c r="C3" s="32" t="s">
-        <v>454</v>
-      </c>
-      <c r="D3" s="32" t="s">
-        <v>353</v>
-      </c>
-      <c r="E3" s="32">
-        <v>4656</v>
-      </c>
-      <c r="F3" s="32" t="s">
-        <v>481</v>
-      </c>
-      <c r="G3" s="32" t="s">
-        <v>467</v>
-      </c>
-      <c r="H3" s="32" t="s">
-        <v>390</v>
-      </c>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32" t="s">
-        <v>276</v>
-      </c>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
-      <c r="O3" s="32"/>
-    </row>
-    <row r="4" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="32" t="s">
-        <v>482</v>
-      </c>
-      <c r="B4" s="32" t="s">
-        <v>495</v>
-      </c>
-      <c r="C4" s="32" t="s">
-        <v>454</v>
-      </c>
-      <c r="D4" s="32" t="s">
-        <v>353</v>
-      </c>
-      <c r="E4" s="32">
-        <v>4656</v>
-      </c>
-      <c r="F4" s="32" t="s">
-        <v>483</v>
-      </c>
-      <c r="G4" s="32" t="s">
-        <v>467</v>
-      </c>
-      <c r="H4" s="32" t="s">
-        <v>390</v>
-      </c>
-      <c r="I4" s="32" t="s">
-        <v>484</v>
-      </c>
-      <c r="J4" s="32" t="s">
-        <v>276</v>
-      </c>
-      <c r="K4" s="32"/>
-      <c r="L4" s="32"/>
-      <c r="M4" s="32"/>
-      <c r="N4" s="32"/>
-      <c r="O4" s="32"/>
-    </row>
-    <row r="5" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="32" t="s">
-        <v>485</v>
-      </c>
-      <c r="B5" s="32" t="s">
-        <v>495</v>
-      </c>
-      <c r="C5" s="32" t="s">
-        <v>454</v>
-      </c>
-      <c r="D5" s="32" t="s">
-        <v>353</v>
-      </c>
-      <c r="E5" s="32">
-        <v>4656</v>
-      </c>
-      <c r="F5" s="32" t="s">
-        <v>481</v>
-      </c>
-      <c r="G5" s="32" t="s">
-        <v>467</v>
-      </c>
-      <c r="H5" s="32" t="s">
-        <v>390</v>
-      </c>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32" t="s">
-        <v>276</v>
-      </c>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="32"/>
-      <c r="O5" s="32"/>
-    </row>
-    <row r="6" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="32" t="s">
-        <v>486</v>
-      </c>
-      <c r="B6" s="32" t="s">
-        <v>495</v>
-      </c>
-      <c r="C6" s="32" t="s">
-        <v>454</v>
-      </c>
-      <c r="D6" s="32" t="s">
-        <v>353</v>
-      </c>
-      <c r="E6" s="32">
-        <v>4656</v>
-      </c>
-      <c r="F6" s="32" t="s">
-        <v>481</v>
-      </c>
-      <c r="G6" s="32" t="s">
-        <v>467</v>
-      </c>
-      <c r="H6" s="32" t="s">
-        <v>390</v>
-      </c>
-      <c r="I6" s="32" t="s">
-        <v>487</v>
-      </c>
-      <c r="J6" s="32" t="s">
-        <v>276</v>
-      </c>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="32"/>
-      <c r="O6" s="32"/>
-    </row>
-    <row r="7" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="32" t="s">
-        <v>488</v>
-      </c>
-      <c r="B7" s="32" t="s">
-        <v>495</v>
-      </c>
-      <c r="C7" s="32" t="s">
-        <v>454</v>
-      </c>
-      <c r="D7" s="32" t="s">
-        <v>353</v>
-      </c>
-      <c r="E7" s="32">
-        <v>4656</v>
-      </c>
-      <c r="F7" s="32" t="s">
-        <v>481</v>
-      </c>
-      <c r="G7" s="32" t="s">
-        <v>467</v>
-      </c>
-      <c r="H7" s="32" t="s">
-        <v>390</v>
-      </c>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32" t="s">
-        <v>276</v>
-      </c>
-      <c r="K7" s="32"/>
-      <c r="L7" s="32" t="s">
-        <v>489</v>
-      </c>
-      <c r="M7" s="32"/>
-      <c r="N7" s="32"/>
-      <c r="O7" s="32"/>
-    </row>
-    <row r="8" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="32" t="s">
-        <v>490</v>
-      </c>
-      <c r="B8" s="32" t="s">
-        <v>495</v>
-      </c>
-      <c r="C8" s="32" t="s">
-        <v>454</v>
-      </c>
-      <c r="D8" s="32" t="s">
-        <v>353</v>
-      </c>
-      <c r="E8" s="32">
-        <v>4656</v>
-      </c>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32" t="s">
-        <v>467</v>
-      </c>
-      <c r="H8" s="32" t="s">
-        <v>390</v>
-      </c>
-      <c r="I8" s="32" t="s">
-        <v>491</v>
-      </c>
-      <c r="J8" s="32" t="s">
-        <v>276</v>
-      </c>
-      <c r="K8" s="32" t="s">
-        <v>492</v>
-      </c>
-      <c r="L8" s="32"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="32"/>
-      <c r="O8" s="32"/>
-    </row>
-    <row r="9" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="32" t="s">
-        <v>493</v>
-      </c>
-      <c r="B9" s="32" t="s">
-        <v>495</v>
-      </c>
-      <c r="C9" s="32" t="s">
-        <v>454</v>
-      </c>
-      <c r="D9" s="32" t="s">
-        <v>353</v>
-      </c>
-      <c r="E9" s="32">
-        <v>4656</v>
-      </c>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32" t="s">
-        <v>467</v>
-      </c>
-      <c r="H9" s="32" t="s">
-        <v>390</v>
-      </c>
-      <c r="I9" s="32" t="s">
-        <v>494</v>
-      </c>
-      <c r="J9" s="32" t="s">
-        <v>276</v>
-      </c>
-      <c r="K9" s="32"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="32"/>
-      <c r="O9" s="32"/>
-    </row>
-    <row r="10" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
21/11/2017 - Cardholder module update for config update
</commit_message>
<xml_diff>
--- a/src/main/resources/config/stage/TestData/TestData.xlsx
+++ b/src/main/resources/config/stage/TestData/TestData.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1899" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1934" uniqueCount="609">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -1711,9 +1711,6 @@
     <t>TC_LoginCardholderPortal</t>
   </si>
   <si>
-    <t>TC_viewChargeForRefundOnWalletClosure</t>
-  </si>
-  <si>
     <t>10000173090000012</t>
   </si>
   <si>
@@ -1723,9 +1720,6 @@
     <t>TC_masterCardMoneyTransfer</t>
   </si>
   <si>
-    <t>4564564564654654564</t>
-  </si>
-  <si>
     <t>Tester</t>
   </si>
   <si>
@@ -1801,9 +1795,6 @@
     <t>TC_cashRemittanceBookting</t>
   </si>
   <si>
-    <t>000000070</t>
-  </si>
-  <si>
     <t>TEST</t>
   </si>
   <si>
@@ -1844,6 +1835,27 @@
   </si>
   <si>
     <t>TC_activationLifeLongForInternationalUse</t>
+  </si>
+  <si>
+    <t>TC_ViewChargeForFundTransfer</t>
+  </si>
+  <si>
+    <t>TC_ViewChargeForWalletToWalletDebit</t>
+  </si>
+  <si>
+    <t>TC_ViewChargeForWalletClosure</t>
+  </si>
+  <si>
+    <t>TC_ViewChargeForVisaMoneyTransferDebit</t>
+  </si>
+  <si>
+    <t>TC_ViewChargeForIntraBnkWalletToWalletTransferDebit</t>
+  </si>
+  <si>
+    <t>TC_ViewChargeForMasterCardMoneySend</t>
+  </si>
+  <si>
+    <t>10000117311000005</t>
   </si>
 </sst>
 </file>
@@ -1953,7 +1965,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -2030,6 +2042,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -9309,10 +9328,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BC20"/>
+  <dimension ref="A1:BC27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9544,7 +9563,7 @@
         <v>550</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>552</v>
@@ -9629,7 +9648,7 @@
         <v>550</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>552</v>
@@ -9693,16 +9712,16 @@
     </row>
     <row r="4" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>560</v>
+        <v>602</v>
       </c>
       <c r="B4" s="39" t="s">
         <v>549</v>
       </c>
       <c r="C4" s="9" t="s">
+        <v>560</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>561</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>562</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>552</v>
@@ -9766,7 +9785,7 @@
     </row>
     <row r="5" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B5" s="39" t="s">
         <v>549</v>
@@ -9775,7 +9794,7 @@
         <v>550</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>552</v>
@@ -9790,7 +9809,7 @@
         <v>554</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>564</v>
+        <v>608</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>556</v>
@@ -9802,13 +9821,13 @@
         <v>955689456</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>566</v>
-      </c>
-      <c r="O5" t="s">
-        <v>551</v>
+        <v>564</v>
+      </c>
+      <c r="O5" s="48" t="s">
+        <v>561</v>
       </c>
       <c r="P5" s="2" t="s">
         <v>555</v>
@@ -9855,7 +9874,7 @@
     </row>
     <row r="6" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="B6" s="39" t="s">
         <v>549</v>
@@ -9864,7 +9883,7 @@
         <v>550</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>552</v>
@@ -9928,7 +9947,7 @@
     </row>
     <row r="7" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="B7" s="39" t="s">
         <v>549</v>
@@ -9937,7 +9956,7 @@
         <v>550</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>552</v>
@@ -9967,10 +9986,10 @@
         <v>10</v>
       </c>
       <c r="V7" s="9" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="X7" s="2"/>
       <c r="Y7" s="2"/>
@@ -10007,7 +10026,7 @@
     </row>
     <row r="8" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B8" s="39" t="s">
         <v>549</v>
@@ -10016,7 +10035,7 @@
         <v>550</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>552</v>
@@ -10046,16 +10065,16 @@
         <v>10</v>
       </c>
       <c r="V8" s="9" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="W8" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="X8" s="2" t="s">
         <v>570</v>
       </c>
-      <c r="X8" s="2" t="s">
-        <v>572</v>
-      </c>
       <c r="Y8" s="40" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="Z8" s="2"/>
       <c r="AA8" s="2"/>
@@ -10090,7 +10109,7 @@
     </row>
     <row r="9" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="B9" s="39" t="s">
         <v>549</v>
@@ -10099,7 +10118,7 @@
         <v>550</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>552</v>
@@ -10129,28 +10148,28 @@
         <v>10</v>
       </c>
       <c r="V9" s="9" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="W9" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="X9" s="2" t="s">
         <v>570</v>
       </c>
-      <c r="X9" s="2" t="s">
-        <v>572</v>
-      </c>
       <c r="Y9" s="40" t="s">
+        <v>571</v>
+      </c>
+      <c r="Z9" s="40" t="s">
         <v>573</v>
       </c>
-      <c r="Z9" s="40" t="s">
+      <c r="AA9" s="40" t="s">
+        <v>574</v>
+      </c>
+      <c r="AB9" s="2" t="s">
         <v>575</v>
       </c>
-      <c r="AA9" s="40" t="s">
+      <c r="AC9" s="2" t="s">
         <v>576</v>
-      </c>
-      <c r="AB9" s="2" t="s">
-        <v>577</v>
-      </c>
-      <c r="AC9" s="2" t="s">
-        <v>578</v>
       </c>
       <c r="AD9" s="2"/>
       <c r="AE9" s="2"/>
@@ -10181,7 +10200,7 @@
     </row>
     <row r="10" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="B10" s="39" t="s">
         <v>549</v>
@@ -10190,7 +10209,7 @@
         <v>550</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>552</v>
@@ -10220,28 +10239,28 @@
         <v>10</v>
       </c>
       <c r="V10" s="9" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="W10" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="X10" s="2" t="s">
         <v>570</v>
       </c>
-      <c r="X10" s="2" t="s">
-        <v>572</v>
-      </c>
       <c r="Y10" s="40" t="s">
+        <v>571</v>
+      </c>
+      <c r="Z10" s="40" t="s">
         <v>573</v>
       </c>
-      <c r="Z10" s="40" t="s">
+      <c r="AA10" s="40" t="s">
+        <v>574</v>
+      </c>
+      <c r="AB10" s="2" t="s">
         <v>575</v>
       </c>
-      <c r="AA10" s="40" t="s">
+      <c r="AC10" s="2" t="s">
         <v>576</v>
-      </c>
-      <c r="AB10" s="2" t="s">
-        <v>577</v>
-      </c>
-      <c r="AC10" s="2" t="s">
-        <v>578</v>
       </c>
       <c r="AD10" s="2"/>
       <c r="AE10" s="2"/>
@@ -10272,7 +10291,7 @@
     </row>
     <row r="11" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="B11" s="39" t="s">
         <v>549</v>
@@ -10281,7 +10300,7 @@
         <v>550</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>552</v>
@@ -10311,38 +10330,38 @@
         <v>10</v>
       </c>
       <c r="V11" s="9" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="W11" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="X11" s="2" t="s">
         <v>570</v>
       </c>
-      <c r="X11" s="2" t="s">
-        <v>572</v>
-      </c>
       <c r="Y11" s="40" t="s">
+        <v>571</v>
+      </c>
+      <c r="Z11" s="40" t="s">
         <v>573</v>
       </c>
-      <c r="Z11" s="40" t="s">
+      <c r="AA11" s="40" t="s">
+        <v>574</v>
+      </c>
+      <c r="AB11" s="2" t="s">
         <v>575</v>
       </c>
-      <c r="AA11" s="40" t="s">
+      <c r="AC11" s="2" t="s">
         <v>576</v>
       </c>
-      <c r="AB11" s="2" t="s">
-        <v>577</v>
-      </c>
-      <c r="AC11" s="2" t="s">
-        <v>578</v>
-      </c>
       <c r="AD11" s="2" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="AE11" s="2"/>
       <c r="AF11" s="2" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="AG11" s="2" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="AH11" s="2"/>
       <c r="AI11" s="2"/>
@@ -10369,7 +10388,7 @@
     </row>
     <row r="12" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B12" s="39" t="s">
         <v>549</v>
@@ -10378,7 +10397,7 @@
         <v>550</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>552</v>
@@ -10408,38 +10427,38 @@
         <v>10</v>
       </c>
       <c r="V12" s="9" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="W12" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="X12" s="2" t="s">
         <v>570</v>
       </c>
-      <c r="X12" s="2" t="s">
-        <v>572</v>
-      </c>
       <c r="Y12" s="40" t="s">
+        <v>571</v>
+      </c>
+      <c r="Z12" s="40" t="s">
         <v>573</v>
       </c>
-      <c r="Z12" s="40" t="s">
+      <c r="AA12" s="40" t="s">
+        <v>574</v>
+      </c>
+      <c r="AB12" s="2" t="s">
         <v>575</v>
       </c>
-      <c r="AA12" s="40" t="s">
+      <c r="AC12" s="2" t="s">
         <v>576</v>
-      </c>
-      <c r="AB12" s="2" t="s">
-        <v>577</v>
-      </c>
-      <c r="AC12" s="2" t="s">
-        <v>578</v>
       </c>
       <c r="AD12" s="2"/>
       <c r="AE12" s="2" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="AF12" s="2" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="AG12" s="2" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="AH12" s="2"/>
       <c r="AI12" s="2"/>
@@ -10466,7 +10485,7 @@
     </row>
     <row r="13" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="B13" s="39" t="s">
         <v>549</v>
@@ -10475,7 +10494,7 @@
         <v>550</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>552</v>
@@ -10505,41 +10524,41 @@
         <v>10</v>
       </c>
       <c r="V13" s="9" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="W13" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="X13" s="2" t="s">
         <v>570</v>
       </c>
-      <c r="X13" s="2" t="s">
-        <v>572</v>
-      </c>
       <c r="Y13" s="40" t="s">
+        <v>571</v>
+      </c>
+      <c r="Z13" s="40" t="s">
         <v>573</v>
       </c>
-      <c r="Z13" s="40" t="s">
+      <c r="AA13" s="40" t="s">
+        <v>574</v>
+      </c>
+      <c r="AB13" s="2" t="s">
         <v>575</v>
       </c>
-      <c r="AA13" s="40" t="s">
+      <c r="AC13" s="2" t="s">
         <v>576</v>
-      </c>
-      <c r="AB13" s="2" t="s">
-        <v>577</v>
-      </c>
-      <c r="AC13" s="2" t="s">
-        <v>578</v>
       </c>
       <c r="AD13" s="2"/>
       <c r="AE13" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="AF13" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="AG13" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="AH13" s="40" t="s">
         <v>584</v>
-      </c>
-      <c r="AF13" s="2" t="s">
-        <v>582</v>
-      </c>
-      <c r="AG13" s="2" t="s">
-        <v>582</v>
-      </c>
-      <c r="AH13" s="40" t="s">
-        <v>586</v>
       </c>
       <c r="AI13" s="2"/>
       <c r="AJ13" s="2"/>
@@ -10565,7 +10584,7 @@
     </row>
     <row r="14" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="B14" s="39" t="s">
         <v>549</v>
@@ -10574,7 +10593,7 @@
         <v>550</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>552</v>
@@ -10604,41 +10623,41 @@
         <v>10</v>
       </c>
       <c r="V14" s="9" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="W14" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="X14" s="2" t="s">
         <v>570</v>
       </c>
-      <c r="X14" s="2" t="s">
-        <v>572</v>
-      </c>
       <c r="Y14" s="40" t="s">
+        <v>571</v>
+      </c>
+      <c r="Z14" s="40" t="s">
         <v>573</v>
       </c>
-      <c r="Z14" s="40" t="s">
+      <c r="AA14" s="40" t="s">
+        <v>574</v>
+      </c>
+      <c r="AB14" s="2" t="s">
         <v>575</v>
       </c>
-      <c r="AA14" s="40" t="s">
+      <c r="AC14" s="2" t="s">
         <v>576</v>
-      </c>
-      <c r="AB14" s="2" t="s">
-        <v>577</v>
-      </c>
-      <c r="AC14" s="2" t="s">
-        <v>578</v>
       </c>
       <c r="AD14" s="2"/>
       <c r="AE14" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="AF14" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="AG14" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="AH14" s="40" t="s">
         <v>584</v>
-      </c>
-      <c r="AF14" s="2" t="s">
-        <v>582</v>
-      </c>
-      <c r="AG14" s="2" t="s">
-        <v>582</v>
-      </c>
-      <c r="AH14" s="40" t="s">
-        <v>586</v>
       </c>
       <c r="AI14" s="2"/>
       <c r="AJ14" s="2"/>
@@ -10664,7 +10683,7 @@
     </row>
     <row r="15" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="B15" s="39" t="s">
         <v>549</v>
@@ -10673,7 +10692,7 @@
         <v>550</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>552</v>
@@ -10703,41 +10722,41 @@
         <v>10</v>
       </c>
       <c r="V15" s="9" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="W15" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="X15" s="2" t="s">
         <v>570</v>
       </c>
-      <c r="X15" s="2" t="s">
-        <v>572</v>
-      </c>
       <c r="Y15" s="40" t="s">
+        <v>571</v>
+      </c>
+      <c r="Z15" s="40" t="s">
         <v>573</v>
       </c>
-      <c r="Z15" s="40" t="s">
+      <c r="AA15" s="40" t="s">
+        <v>574</v>
+      </c>
+      <c r="AB15" s="2" t="s">
         <v>575</v>
       </c>
-      <c r="AA15" s="40" t="s">
+      <c r="AC15" s="2" t="s">
         <v>576</v>
-      </c>
-      <c r="AB15" s="2" t="s">
-        <v>577</v>
-      </c>
-      <c r="AC15" s="2" t="s">
-        <v>578</v>
       </c>
       <c r="AD15" s="2"/>
       <c r="AE15" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="AF15" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="AG15" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="AH15" s="40" t="s">
         <v>584</v>
-      </c>
-      <c r="AF15" s="2" t="s">
-        <v>582</v>
-      </c>
-      <c r="AG15" s="2" t="s">
-        <v>582</v>
-      </c>
-      <c r="AH15" s="40" t="s">
-        <v>586</v>
       </c>
       <c r="AI15" s="2"/>
       <c r="AJ15" s="2"/>
@@ -10763,16 +10782,16 @@
     </row>
     <row r="16" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="B16" s="39" t="s">
         <v>549</v>
       </c>
       <c r="C16" s="9" t="s">
+        <v>560</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>561</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>590</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>552</v>
@@ -10813,31 +10832,31 @@
       <c r="AG16" s="2"/>
       <c r="AH16" s="2"/>
       <c r="AI16" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="AJ16" s="2" t="s">
+        <v>589</v>
+      </c>
+      <c r="AK16" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="AL16" s="2" t="s">
         <v>591</v>
       </c>
-      <c r="AJ16" s="2" t="s">
+      <c r="AM16" s="2" t="s">
         <v>592</v>
       </c>
-      <c r="AK16" s="2" t="s">
+      <c r="AN16" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="AO16" s="2" t="s">
         <v>593</v>
       </c>
-      <c r="AL16" s="2" t="s">
+      <c r="AP16" s="2" t="s">
         <v>594</v>
       </c>
-      <c r="AM16" s="2" t="s">
+      <c r="AQ16" s="2" t="s">
         <v>595</v>
-      </c>
-      <c r="AN16" s="2" t="s">
-        <v>595</v>
-      </c>
-      <c r="AO16" s="2" t="s">
-        <v>596</v>
-      </c>
-      <c r="AP16" s="2" t="s">
-        <v>597</v>
-      </c>
-      <c r="AQ16" s="2" t="s">
-        <v>598</v>
       </c>
       <c r="AR16" s="2" t="s">
         <v>30</v>
@@ -10846,7 +10865,7 @@
         <v>411033</v>
       </c>
       <c r="AT16" s="41" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="AU16" s="2">
         <v>7896543215</v>
@@ -10855,7 +10874,7 @@
         <v>5000</v>
       </c>
       <c r="AW16" s="2" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="AX16" s="2"/>
       <c r="AY16" s="2"/>
@@ -10866,7 +10885,7 @@
     </row>
     <row r="17" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="B17" s="39" t="s">
         <v>549</v>
@@ -10875,7 +10894,7 @@
         <v>550</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>552</v>
@@ -10916,31 +10935,31 @@
       <c r="AG17" s="2"/>
       <c r="AH17" s="2"/>
       <c r="AI17" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="AJ17" s="2" t="s">
+        <v>589</v>
+      </c>
+      <c r="AK17" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="AL17" s="2" t="s">
         <v>591</v>
       </c>
-      <c r="AJ17" s="2" t="s">
+      <c r="AM17" s="2" t="s">
         <v>592</v>
       </c>
-      <c r="AK17" s="2" t="s">
+      <c r="AN17" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="AO17" s="2" t="s">
         <v>593</v>
       </c>
-      <c r="AL17" s="2" t="s">
+      <c r="AP17" s="2" t="s">
         <v>594</v>
       </c>
-      <c r="AM17" s="2" t="s">
+      <c r="AQ17" s="2" t="s">
         <v>595</v>
-      </c>
-      <c r="AN17" s="2" t="s">
-        <v>595</v>
-      </c>
-      <c r="AO17" s="2" t="s">
-        <v>596</v>
-      </c>
-      <c r="AP17" s="2" t="s">
-        <v>597</v>
-      </c>
-      <c r="AQ17" s="2" t="s">
-        <v>598</v>
       </c>
       <c r="AR17" s="2" t="s">
         <v>30</v>
@@ -10949,7 +10968,7 @@
         <v>411033</v>
       </c>
       <c r="AT17" s="41" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="AU17" s="2">
         <v>7896543215</v>
@@ -10958,13 +10977,13 @@
         <v>5000</v>
       </c>
       <c r="AW17" s="2" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="AX17" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="AY17" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="AZ17" s="2"/>
       <c r="BA17" s="2"/>
@@ -10973,7 +10992,7 @@
     </row>
     <row r="18" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="B18" s="39" t="s">
         <v>549</v>
@@ -10982,7 +11001,7 @@
         <v>550</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>552</v>
@@ -11023,31 +11042,31 @@
       <c r="AG18" s="2"/>
       <c r="AH18" s="2"/>
       <c r="AI18" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="AJ18" s="2" t="s">
+        <v>589</v>
+      </c>
+      <c r="AK18" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="AL18" s="2" t="s">
         <v>591</v>
       </c>
-      <c r="AJ18" s="2" t="s">
+      <c r="AM18" s="2" t="s">
         <v>592</v>
       </c>
-      <c r="AK18" s="2" t="s">
+      <c r="AN18" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="AO18" s="2" t="s">
         <v>593</v>
       </c>
-      <c r="AL18" s="2" t="s">
+      <c r="AP18" s="2" t="s">
         <v>594</v>
       </c>
-      <c r="AM18" s="2" t="s">
+      <c r="AQ18" s="2" t="s">
         <v>595</v>
-      </c>
-      <c r="AN18" s="2" t="s">
-        <v>595</v>
-      </c>
-      <c r="AO18" s="2" t="s">
-        <v>596</v>
-      </c>
-      <c r="AP18" s="2" t="s">
-        <v>597</v>
-      </c>
-      <c r="AQ18" s="2" t="s">
-        <v>598</v>
       </c>
       <c r="AR18" s="2" t="s">
         <v>30</v>
@@ -11056,7 +11075,7 @@
         <v>411033</v>
       </c>
       <c r="AT18" s="41" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="AU18" s="2">
         <v>7896543215</v>
@@ -11065,13 +11084,13 @@
         <v>5000</v>
       </c>
       <c r="AW18" s="2" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="AX18" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="AY18" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="AZ18" s="2"/>
       <c r="BA18" s="2"/>
@@ -11080,7 +11099,7 @@
     </row>
     <row r="19" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="B19" s="39" t="s">
         <v>549</v>
@@ -11089,7 +11108,7 @@
         <v>550</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>552</v>
@@ -11130,31 +11149,31 @@
       <c r="AG19" s="2"/>
       <c r="AH19" s="2"/>
       <c r="AI19" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="AJ19" s="2" t="s">
+        <v>589</v>
+      </c>
+      <c r="AK19" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="AL19" s="2" t="s">
         <v>591</v>
       </c>
-      <c r="AJ19" s="2" t="s">
+      <c r="AM19" s="2" t="s">
         <v>592</v>
       </c>
-      <c r="AK19" s="2" t="s">
+      <c r="AN19" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="AO19" s="2" t="s">
         <v>593</v>
       </c>
-      <c r="AL19" s="2" t="s">
+      <c r="AP19" s="2" t="s">
         <v>594</v>
       </c>
-      <c r="AM19" s="2" t="s">
+      <c r="AQ19" s="2" t="s">
         <v>595</v>
-      </c>
-      <c r="AN19" s="2" t="s">
-        <v>595</v>
-      </c>
-      <c r="AO19" s="2" t="s">
-        <v>596</v>
-      </c>
-      <c r="AP19" s="2" t="s">
-        <v>597</v>
-      </c>
-      <c r="AQ19" s="2" t="s">
-        <v>598</v>
       </c>
       <c r="AR19" s="2" t="s">
         <v>30</v>
@@ -11163,7 +11182,7 @@
         <v>411033</v>
       </c>
       <c r="AT19" s="41" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="AU19" s="2">
         <v>7896543215</v>
@@ -11172,13 +11191,13 @@
         <v>5000</v>
       </c>
       <c r="AW19" s="2" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="AX19" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="AY19" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="AZ19" s="2"/>
       <c r="BA19" s="2"/>
@@ -11187,7 +11206,7 @@
     </row>
     <row r="20" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="B20" s="39" t="s">
         <v>549</v>
@@ -11196,7 +11215,7 @@
         <v>550</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>552</v>
@@ -11237,31 +11256,31 @@
       <c r="AG20" s="2"/>
       <c r="AH20" s="2"/>
       <c r="AI20" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="AJ20" s="2" t="s">
+        <v>589</v>
+      </c>
+      <c r="AK20" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="AL20" s="2" t="s">
         <v>591</v>
       </c>
-      <c r="AJ20" s="2" t="s">
+      <c r="AM20" s="2" t="s">
         <v>592</v>
       </c>
-      <c r="AK20" s="2" t="s">
+      <c r="AN20" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="AO20" s="2" t="s">
         <v>593</v>
       </c>
-      <c r="AL20" s="2" t="s">
+      <c r="AP20" s="2" t="s">
         <v>594</v>
       </c>
-      <c r="AM20" s="2" t="s">
+      <c r="AQ20" s="2" t="s">
         <v>595</v>
-      </c>
-      <c r="AN20" s="2" t="s">
-        <v>595</v>
-      </c>
-      <c r="AO20" s="2" t="s">
-        <v>596</v>
-      </c>
-      <c r="AP20" s="2" t="s">
-        <v>597</v>
-      </c>
-      <c r="AQ20" s="2" t="s">
-        <v>598</v>
       </c>
       <c r="AR20" s="2" t="s">
         <v>30</v>
@@ -11270,7 +11289,7 @@
         <v>411033</v>
       </c>
       <c r="AT20" s="41" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="AU20" s="2">
         <v>7896543215</v>
@@ -11279,18 +11298,497 @@
         <v>5000</v>
       </c>
       <c r="AW20" s="2" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="AX20" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="AY20" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="AZ20" s="2"/>
       <c r="BA20" s="2"/>
       <c r="BB20" s="2"/>
       <c r="BC20" s="2"/>
+    </row>
+    <row r="21" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="B21" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>560</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>561</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F21" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="2"/>
+      <c r="U21" s="2"/>
+      <c r="V21" s="9"/>
+      <c r="W21" s="2"/>
+      <c r="X21" s="2"/>
+      <c r="Y21" s="2"/>
+      <c r="Z21" s="2"/>
+      <c r="AA21" s="2"/>
+      <c r="AB21" s="2"/>
+      <c r="AC21" s="2"/>
+      <c r="AD21" s="2"/>
+      <c r="AE21" s="2"/>
+      <c r="AF21" s="2"/>
+      <c r="AG21" s="2"/>
+      <c r="AH21" s="2"/>
+      <c r="AI21" s="2"/>
+      <c r="AJ21" s="2"/>
+      <c r="AK21" s="2"/>
+      <c r="AL21" s="2"/>
+      <c r="AM21" s="2"/>
+      <c r="AN21" s="2"/>
+      <c r="AO21" s="2"/>
+      <c r="AP21" s="2"/>
+      <c r="AQ21" s="2"/>
+      <c r="AR21" s="2"/>
+      <c r="AS21" s="2"/>
+      <c r="AT21" s="2"/>
+      <c r="AU21" s="2"/>
+      <c r="AV21" s="2"/>
+      <c r="AW21" s="2"/>
+      <c r="AX21" s="2"/>
+      <c r="AY21" s="2"/>
+      <c r="AZ21" s="2"/>
+      <c r="BA21" s="2"/>
+      <c r="BB21" s="2"/>
+      <c r="BC21" s="2"/>
+    </row>
+    <row r="22" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="B22" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>560</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>561</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F22" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2"/>
+      <c r="V22" s="9"/>
+      <c r="W22" s="2"/>
+      <c r="X22" s="2"/>
+      <c r="Y22" s="2"/>
+      <c r="Z22" s="2"/>
+      <c r="AA22" s="2"/>
+      <c r="AB22" s="2"/>
+      <c r="AC22" s="2"/>
+      <c r="AD22" s="2"/>
+      <c r="AE22" s="2"/>
+      <c r="AF22" s="2"/>
+      <c r="AG22" s="2"/>
+      <c r="AH22" s="2"/>
+      <c r="AI22" s="2"/>
+      <c r="AJ22" s="2"/>
+      <c r="AK22" s="2"/>
+      <c r="AL22" s="2"/>
+      <c r="AM22" s="2"/>
+      <c r="AN22" s="2"/>
+      <c r="AO22" s="2"/>
+      <c r="AP22" s="2"/>
+      <c r="AQ22" s="2"/>
+      <c r="AR22" s="2"/>
+      <c r="AS22" s="2"/>
+      <c r="AT22" s="2"/>
+      <c r="AU22" s="2"/>
+      <c r="AV22" s="2"/>
+      <c r="AW22" s="2"/>
+      <c r="AX22" s="2"/>
+      <c r="AY22" s="2"/>
+      <c r="AZ22" s="2"/>
+      <c r="BA22" s="2"/>
+      <c r="BB22" s="2"/>
+      <c r="BC22" s="2"/>
+    </row>
+    <row r="23" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="B23" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>560</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>561</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F23" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="9"/>
+      <c r="W23" s="2"/>
+      <c r="X23" s="2"/>
+      <c r="Y23" s="2"/>
+      <c r="Z23" s="2"/>
+      <c r="AA23" s="2"/>
+      <c r="AB23" s="2"/>
+      <c r="AC23" s="2"/>
+      <c r="AD23" s="2"/>
+      <c r="AE23" s="2"/>
+      <c r="AF23" s="2"/>
+      <c r="AG23" s="2"/>
+      <c r="AH23" s="2"/>
+      <c r="AI23" s="2"/>
+      <c r="AJ23" s="2"/>
+      <c r="AK23" s="2"/>
+      <c r="AL23" s="2"/>
+      <c r="AM23" s="2"/>
+      <c r="AN23" s="2"/>
+      <c r="AO23" s="2"/>
+      <c r="AP23" s="2"/>
+      <c r="AQ23" s="2"/>
+      <c r="AR23" s="2"/>
+      <c r="AS23" s="2"/>
+      <c r="AT23" s="2"/>
+      <c r="AU23" s="2"/>
+      <c r="AV23" s="2"/>
+      <c r="AW23" s="2"/>
+      <c r="AX23" s="2"/>
+      <c r="AY23" s="2"/>
+      <c r="AZ23" s="2"/>
+      <c r="BA23" s="2"/>
+      <c r="BB23" s="2"/>
+      <c r="BC23" s="2"/>
+    </row>
+    <row r="24" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="B24" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>560</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>561</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F24" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+      <c r="S24" s="2"/>
+      <c r="T24" s="2"/>
+      <c r="U24" s="2"/>
+      <c r="V24" s="9"/>
+      <c r="W24" s="2"/>
+      <c r="X24" s="2"/>
+      <c r="Y24" s="2"/>
+      <c r="Z24" s="2"/>
+      <c r="AA24" s="2"/>
+      <c r="AB24" s="2"/>
+      <c r="AC24" s="2"/>
+      <c r="AD24" s="2"/>
+      <c r="AE24" s="2"/>
+      <c r="AF24" s="2"/>
+      <c r="AG24" s="2"/>
+      <c r="AH24" s="2"/>
+      <c r="AI24" s="2"/>
+      <c r="AJ24" s="2"/>
+      <c r="AK24" s="2"/>
+      <c r="AL24" s="2"/>
+      <c r="AM24" s="2"/>
+      <c r="AN24" s="2"/>
+      <c r="AO24" s="2"/>
+      <c r="AP24" s="2"/>
+      <c r="AQ24" s="2"/>
+      <c r="AR24" s="2"/>
+      <c r="AS24" s="2"/>
+      <c r="AT24" s="2"/>
+      <c r="AU24" s="2"/>
+      <c r="AV24" s="2"/>
+      <c r="AW24" s="2"/>
+      <c r="AX24" s="2"/>
+      <c r="AY24" s="2"/>
+      <c r="AZ24" s="2"/>
+      <c r="BA24" s="2"/>
+      <c r="BB24" s="2"/>
+      <c r="BC24" s="2"/>
+    </row>
+    <row r="25" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="B25" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>560</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>561</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F25" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2"/>
+      <c r="U25" s="2"/>
+      <c r="V25" s="9"/>
+      <c r="W25" s="2"/>
+      <c r="X25" s="2"/>
+      <c r="Y25" s="2"/>
+      <c r="Z25" s="2"/>
+      <c r="AA25" s="2"/>
+      <c r="AB25" s="2"/>
+      <c r="AC25" s="2"/>
+      <c r="AD25" s="2"/>
+      <c r="AE25" s="2"/>
+      <c r="AF25" s="2"/>
+      <c r="AG25" s="2"/>
+      <c r="AH25" s="2"/>
+      <c r="AI25" s="2"/>
+      <c r="AJ25" s="2"/>
+      <c r="AK25" s="2"/>
+      <c r="AL25" s="2"/>
+      <c r="AM25" s="2"/>
+      <c r="AN25" s="2"/>
+      <c r="AO25" s="2"/>
+      <c r="AP25" s="2"/>
+      <c r="AQ25" s="2"/>
+      <c r="AR25" s="2"/>
+      <c r="AS25" s="2"/>
+      <c r="AT25" s="2"/>
+      <c r="AU25" s="2"/>
+      <c r="AV25" s="2"/>
+      <c r="AW25" s="2"/>
+      <c r="AX25" s="2"/>
+      <c r="AY25" s="2"/>
+      <c r="AZ25" s="2"/>
+      <c r="BA25" s="2"/>
+      <c r="BB25" s="2"/>
+      <c r="BC25" s="2"/>
+    </row>
+    <row r="26" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A26" s="44"/>
+      <c r="B26" s="45"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="46"/>
+      <c r="I26" s="46"/>
+      <c r="J26" s="46"/>
+      <c r="K26" s="44"/>
+      <c r="L26" s="44"/>
+      <c r="M26" s="44"/>
+      <c r="N26" s="44"/>
+      <c r="O26" s="44"/>
+      <c r="P26" s="44"/>
+      <c r="Q26" s="44"/>
+      <c r="R26" s="44"/>
+      <c r="S26" s="44"/>
+      <c r="T26" s="44"/>
+      <c r="U26" s="44"/>
+      <c r="V26" s="46"/>
+      <c r="W26" s="44"/>
+      <c r="X26" s="44"/>
+      <c r="Y26" s="44"/>
+      <c r="Z26" s="44"/>
+      <c r="AA26" s="44"/>
+      <c r="AB26" s="44"/>
+      <c r="AC26" s="44"/>
+      <c r="AD26" s="44"/>
+      <c r="AE26" s="44"/>
+      <c r="AF26" s="44"/>
+      <c r="AG26" s="44"/>
+      <c r="AH26" s="44"/>
+      <c r="AI26" s="44"/>
+      <c r="AJ26" s="44"/>
+      <c r="AK26" s="44"/>
+      <c r="AL26" s="44"/>
+      <c r="AM26" s="44"/>
+      <c r="AN26" s="44"/>
+      <c r="AO26" s="44"/>
+      <c r="AP26" s="44"/>
+      <c r="AQ26" s="44"/>
+      <c r="AR26" s="44"/>
+      <c r="AS26" s="44"/>
+      <c r="AT26" s="47"/>
+      <c r="AU26" s="44"/>
+      <c r="AV26" s="44"/>
+      <c r="AW26" s="44"/>
+      <c r="AX26" s="44"/>
+      <c r="AY26" s="44"/>
+      <c r="AZ26" s="44"/>
+      <c r="BA26" s="44"/>
+      <c r="BB26" s="44"/>
+      <c r="BC26" s="44"/>
+    </row>
+    <row r="27" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A27" s="44"/>
+      <c r="B27" s="45"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="46"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="46"/>
+      <c r="I27" s="46"/>
+      <c r="J27" s="46"/>
+      <c r="K27" s="44"/>
+      <c r="L27" s="44"/>
+      <c r="M27" s="44"/>
+      <c r="N27" s="44"/>
+      <c r="O27" s="44"/>
+      <c r="P27" s="44"/>
+      <c r="Q27" s="44"/>
+      <c r="R27" s="44"/>
+      <c r="S27" s="44"/>
+      <c r="T27" s="44"/>
+      <c r="U27" s="44"/>
+      <c r="V27" s="46"/>
+      <c r="W27" s="44"/>
+      <c r="X27" s="44"/>
+      <c r="Y27" s="44"/>
+      <c r="Z27" s="44"/>
+      <c r="AA27" s="44"/>
+      <c r="AB27" s="44"/>
+      <c r="AC27" s="44"/>
+      <c r="AD27" s="44"/>
+      <c r="AE27" s="44"/>
+      <c r="AF27" s="44"/>
+      <c r="AG27" s="44"/>
+      <c r="AH27" s="44"/>
+      <c r="AI27" s="44"/>
+      <c r="AJ27" s="44"/>
+      <c r="AK27" s="44"/>
+      <c r="AL27" s="44"/>
+      <c r="AM27" s="44"/>
+      <c r="AN27" s="44"/>
+      <c r="AO27" s="44"/>
+      <c r="AP27" s="44"/>
+      <c r="AQ27" s="44"/>
+      <c r="AR27" s="44"/>
+      <c r="AS27" s="44"/>
+      <c r="AT27" s="47"/>
+      <c r="AU27" s="44"/>
+      <c r="AV27" s="44"/>
+      <c r="AW27" s="44"/>
+      <c r="AX27" s="44"/>
+      <c r="AY27" s="44"/>
+      <c r="AZ27" s="44"/>
+      <c r="BA27" s="44"/>
+      <c r="BB27" s="44"/>
+      <c r="BC27" s="44"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -11318,6 +11816,11 @@
     <hyperlink ref="AT19" r:id="rId22"/>
     <hyperlink ref="B20" r:id="rId23"/>
     <hyperlink ref="AT20" r:id="rId24"/>
+    <hyperlink ref="B21" r:id="rId25"/>
+    <hyperlink ref="B22" r:id="rId26"/>
+    <hyperlink ref="B23" r:id="rId27"/>
+    <hyperlink ref="B24" r:id="rId28"/>
+    <hyperlink ref="B25" r:id="rId29"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
22/11/2017 - Vertual Card script update
</commit_message>
<xml_diff>
--- a/src/main/resources/config/stage/TestData/TestData.xlsx
+++ b/src/main/resources/config/stage/TestData/TestData.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1934" uniqueCount="609">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1941" uniqueCount="610">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -1856,6 +1856,9 @@
   </si>
   <si>
     <t>10000117311000005</t>
+  </si>
+  <si>
+    <t>TC_RequestVirtualPrepaidCard</t>
   </si>
 </sst>
 </file>
@@ -1965,7 +1968,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -2049,6 +2052,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -9330,8 +9334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11677,64 +11681,80 @@
       <c r="BC25" s="2"/>
     </row>
     <row r="26" spans="1:55" x14ac:dyDescent="0.3">
-      <c r="A26" s="44"/>
-      <c r="B26" s="45"/>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="44"/>
-      <c r="F26" s="44"/>
-      <c r="G26" s="44"/>
-      <c r="H26" s="46"/>
-      <c r="I26" s="46"/>
-      <c r="J26" s="46"/>
-      <c r="K26" s="44"/>
-      <c r="L26" s="44"/>
-      <c r="M26" s="44"/>
-      <c r="N26" s="44"/>
-      <c r="O26" s="44"/>
-      <c r="P26" s="44"/>
-      <c r="Q26" s="44"/>
-      <c r="R26" s="44"/>
-      <c r="S26" s="44"/>
-      <c r="T26" s="44"/>
-      <c r="U26" s="44"/>
-      <c r="V26" s="46"/>
-      <c r="W26" s="44"/>
-      <c r="X26" s="44"/>
-      <c r="Y26" s="44"/>
-      <c r="Z26" s="44"/>
-      <c r="AA26" s="44"/>
-      <c r="AB26" s="44"/>
-      <c r="AC26" s="44"/>
-      <c r="AD26" s="44"/>
-      <c r="AE26" s="44"/>
-      <c r="AF26" s="44"/>
-      <c r="AG26" s="44"/>
-      <c r="AH26" s="44"/>
-      <c r="AI26" s="44"/>
-      <c r="AJ26" s="44"/>
-      <c r="AK26" s="44"/>
-      <c r="AL26" s="44"/>
-      <c r="AM26" s="44"/>
-      <c r="AN26" s="44"/>
-      <c r="AO26" s="44"/>
-      <c r="AP26" s="44"/>
-      <c r="AQ26" s="44"/>
-      <c r="AR26" s="44"/>
-      <c r="AS26" s="44"/>
-      <c r="AT26" s="47"/>
-      <c r="AU26" s="44"/>
-      <c r="AV26" s="44"/>
-      <c r="AW26" s="44"/>
-      <c r="AX26" s="44"/>
-      <c r="AY26" s="44"/>
-      <c r="AZ26" s="44"/>
-      <c r="BA26" s="44"/>
-      <c r="BB26" s="44"/>
-      <c r="BC26" s="44"/>
+      <c r="A26" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="B26" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>560</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>561</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F26" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2"/>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2"/>
+      <c r="U26" s="2"/>
+      <c r="V26" s="9"/>
+      <c r="W26" s="2"/>
+      <c r="X26" s="2"/>
+      <c r="Y26" s="2"/>
+      <c r="Z26" s="2"/>
+      <c r="AA26" s="2"/>
+      <c r="AB26" s="2"/>
+      <c r="AC26" s="2"/>
+      <c r="AD26" s="2"/>
+      <c r="AE26" s="2"/>
+      <c r="AF26" s="2"/>
+      <c r="AG26" s="2"/>
+      <c r="AH26" s="2"/>
+      <c r="AI26" s="2"/>
+      <c r="AJ26" s="2"/>
+      <c r="AK26" s="2"/>
+      <c r="AL26" s="2"/>
+      <c r="AM26" s="2"/>
+      <c r="AN26" s="2"/>
+      <c r="AO26" s="2"/>
+      <c r="AP26" s="2"/>
+      <c r="AQ26" s="2"/>
+      <c r="AR26" s="2"/>
+      <c r="AS26" s="2"/>
+      <c r="AT26" s="2"/>
+      <c r="AU26" s="2"/>
+      <c r="AV26" s="2"/>
+      <c r="AW26" s="2"/>
+      <c r="AX26" s="2"/>
+      <c r="AY26" s="2"/>
+      <c r="AZ26" s="2"/>
+      <c r="BA26" s="2"/>
+      <c r="BB26" s="2"/>
+      <c r="BC26" s="2"/>
     </row>
     <row r="27" spans="1:55" x14ac:dyDescent="0.3">
-      <c r="A27" s="44"/>
+      <c r="A27" s="49"/>
       <c r="B27" s="45"/>
       <c r="C27" s="46"/>
       <c r="D27" s="46"/>
@@ -11821,6 +11841,7 @@
     <hyperlink ref="B23" r:id="rId27"/>
     <hyperlink ref="B24" r:id="rId28"/>
     <hyperlink ref="B25" r:id="rId29"/>
+    <hyperlink ref="B26" r:id="rId30"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>